<commit_message>
Delete unnecessary async methods
</commit_message>
<xml_diff>
--- a/Agencies.xlsx
+++ b/Agencies.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Canada Space Agency" sheetId="1" r:id="rId1"/>
+    <sheet name="CSA" sheetId="1" r:id="rId1"/>
+    <sheet name="Roscosmos" sheetId="4" r:id="rId2"/>
+    <sheet name="ISRO" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Budget</t>
   </si>
@@ -72,6 +74,42 @@
   </si>
   <si>
     <t>Ionosphere research</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Shira</t>
+  </si>
+  <si>
+    <t>Solar activity observation</t>
+  </si>
+  <si>
+    <t>Sari</t>
+  </si>
+  <si>
+    <t>Activa</t>
+  </si>
+  <si>
+    <t>Observation of far Universe objects</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Proton</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>ISS supplement and crew delivery</t>
+  </si>
+  <si>
+    <t>Vostok</t>
+  </si>
+  <si>
+    <t>Earth atmosphere observation</t>
   </si>
 </sst>
 </file>
@@ -403,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>37.9</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -499,4 +537,198 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>34611</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>1.58</v>
+      </c>
+      <c r="E2">
+        <v>144.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1">
+        <v>38538</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1">
+        <v>37655</v>
+      </c>
+      <c r="H3" s="1">
+        <v>39756</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>38571</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1360</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1">
+        <v>38968</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41254</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1">
+        <v>42078</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>